<commit_message>
Variables finales. El modelo no predice
</commit_message>
<xml_diff>
--- a/model_03.xlsx
+++ b/model_03.xlsx
@@ -1,21 +1,81 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6abb6dff1a61957e/RProjects/CIS/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_0F65FDCE8F79A8D366075C52F3431AB69713808B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D618CBBE-E540-432B-BDE4-BCB6DC1B6876}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView minimized="1" xWindow="1240" yWindow="-9630" windowWidth="17280" windowHeight="8960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>va</t>
+  </si>
+  <si>
+    <t>co</t>
+  </si>
+  <si>
+    <t>Std_Errors</t>
+  </si>
+  <si>
+    <t>Odds_Ratio</t>
+  </si>
+  <si>
+    <t>(Intercept)</t>
+  </si>
+  <si>
+    <t>SEXO</t>
+  </si>
+  <si>
+    <t>EDAD</t>
+  </si>
+  <si>
+    <t>NIVELESTENTREV</t>
+  </si>
+  <si>
+    <t>SEXO:EDAD</t>
+  </si>
+  <si>
+    <t>SEXO:NIVELESTENTREV</t>
+  </si>
+  <si>
+    <t>Hombre</t>
+  </si>
+  <si>
+    <t>Mujer</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +123,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -107,7 +175,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -141,6 +209,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -175,9 +244,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -350,129 +420,175 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>va</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>co</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Std_Errors</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Odds_Ratio</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>(Intercept)</t>
-        </is>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>-0.775</v>
+        <v>-0.77500000000000002</v>
       </c>
       <c r="C2">
         <v>0.245</v>
       </c>
       <c r="D2">
-        <v>0.461</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>SEXO</t>
-        </is>
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="F2">
+        <f>B2</f>
+        <v>-0.77500000000000002</v>
+      </c>
+      <c r="G2">
+        <f>B2</f>
+        <v>-0.77500000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>-1.828</v>
+        <v>-1.8280000000000001</v>
       </c>
       <c r="C3">
-        <v>0.355</v>
+        <v>0.35499999999999998</v>
       </c>
       <c r="D3">
         <v>0.161</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>EDAD</t>
-        </is>
+      <c r="F3">
+        <f>B3*1</f>
+        <v>-1.8280000000000001</v>
+      </c>
+      <c r="G3">
+        <f>B3*0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>0.003</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C4">
-        <v>0.003</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D4">
-        <v>1.003</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>NIVELESTENTREV</t>
-        </is>
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="F4">
+        <f>B4*50.27</f>
+        <v>0.15081</v>
+      </c>
+      <c r="G4">
+        <f>B4*50.27</f>
+        <v>0.15081</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>-0.044</v>
+        <v>-4.3999999999999997E-2</v>
       </c>
       <c r="C5">
-        <v>0.016</v>
+        <v>1.6E-2</v>
       </c>
       <c r="D5">
-        <v>0.957</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>SEXO:EDAD</t>
-        </is>
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="F5">
+        <f>B5*8.09</f>
+        <v>-0.35596</v>
+      </c>
+      <c r="G5">
+        <f>B5*8.09</f>
+        <v>-0.35596</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>0.017</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="C6">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D6">
-        <v>1.017</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>SEXO:NIVELESTENTREV</t>
-        </is>
+        <v>1.0169999999999999</v>
+      </c>
+      <c r="F6">
+        <f>B6*1*50.27</f>
+        <v>0.85459000000000007</v>
+      </c>
+      <c r="G6">
+        <f>B6*0*50.27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>0.063</v>
+        <v>6.3E-2</v>
       </c>
       <c r="C7">
-        <v>0.023</v>
+        <v>2.3E-2</v>
       </c>
       <c r="D7">
-        <v>1.065</v>
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="F7">
+        <f>B7*1*8.09</f>
+        <v>0.50966999999999996</v>
+      </c>
+      <c r="G7">
+        <f>B7*0*8.09</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <f>SUM(F2:F7)</f>
+        <v>-1.4438900000000006</v>
+      </c>
+      <c r="G8">
+        <f>SUM(G2:G7)</f>
+        <v>-0.98015000000000008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>